<commit_message>
UPD Evich B5 solve 27
</commit_message>
<xml_diff>
--- a/Others_Solutions/Решения из книги Евич/Вариант 5/Задание 26/26.xlsx
+++ b/Others_Solutions/Решения из книги Евич/Вариант 5/Задание 26/26.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hem12\Documents\Документы Миша\Школьные предметы\ЕГЭ информатика\Solutions\PrepareForEGE_MishaPolykovsky\Others_Solutions\Решения из книги Евич\Вариант 5\Задание 26\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CA9762-8542-4286-ABDF-5FD1EF7144B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AE3E4C-C363-43FB-8EAB-ACBBB1840AAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -357,7 +357,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -365,6 +365,9 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>7926</v>
+      </c>
+      <c r="C1">
+        <v>5</v>
       </c>
       <c r="D1">
         <f>SUM(A1:A5)</f>
@@ -442,7 +445,7 @@
   <dimension ref="A1:F9725"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +509,7 @@
         <v>5008</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B5:B68" si="1">IF(OR(A6&lt;&gt;A5, A6&lt;&gt;A7), A6, 0)</f>
+        <f t="shared" ref="B6:B68" si="1">IF(OR(A6&lt;&gt;A5, A6&lt;&gt;A7), A6, 0)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>